<commit_message>
Matlab files updated to newest version
</commit_message>
<xml_diff>
--- a/0_data/T6662_Three_Phase_Reduced.xlsx
+++ b/0_data/T6662_Three_Phase_Reduced.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\48359978\Desktop\T6662_Three_Phase_reduced_function_parallel\0_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FBB8B50-59BE-4814-A982-CBECB961695D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FC77EA1-497B-4327-9405-E6FF84D937FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dg" sheetId="4" r:id="rId1"/>
@@ -505,8 +505,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{039A262C-3198-4C88-87D7-159FCDBC086C}">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -628,7 +628,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="7">
-        <v>826</v>
+        <v>240</v>
       </c>
       <c r="C5" s="7">
         <v>10000</v>
@@ -655,19 +655,19 @@
         <v>5</v>
       </c>
       <c r="B6" s="1">
-        <v>1793</v>
+        <v>250</v>
       </c>
       <c r="C6" s="1">
-        <f>450*2</f>
-        <v>900</v>
+        <f>450*2.5</f>
+        <v>1125</v>
       </c>
       <c r="D6" s="1">
         <f>C6*1</f>
-        <v>900</v>
+        <v>1125</v>
       </c>
       <c r="E6" s="5">
         <f>D6*0.8</f>
-        <v>720</v>
+        <v>900</v>
       </c>
       <c r="F6" s="1">
         <v>2</v>
@@ -684,19 +684,19 @@
         <v>6</v>
       </c>
       <c r="B7" s="1">
-        <v>1212</v>
+        <v>322</v>
       </c>
       <c r="C7" s="1">
-        <f t="shared" ref="C7:C11" si="1">450*2</f>
-        <v>900</v>
+        <f t="shared" ref="C7:C11" si="1">450*2.5</f>
+        <v>1125</v>
       </c>
       <c r="D7" s="1">
         <f>C7*1</f>
-        <v>900</v>
+        <v>1125</v>
       </c>
       <c r="E7" s="1">
         <f t="shared" ref="E7:E33" si="2">D7*0.8</f>
-        <v>720</v>
+        <v>900</v>
       </c>
       <c r="F7" s="1">
         <v>2</v>
@@ -713,19 +713,19 @@
         <v>7</v>
       </c>
       <c r="B8" s="1">
-        <v>485</v>
+        <v>732</v>
       </c>
       <c r="C8" s="1">
         <f t="shared" si="1"/>
-        <v>900</v>
+        <v>1125</v>
       </c>
       <c r="D8" s="1">
         <f>C8</f>
+        <v>1125</v>
+      </c>
+      <c r="E8" s="1">
+        <f t="shared" si="2"/>
         <v>900</v>
-      </c>
-      <c r="E8" s="1">
-        <f t="shared" si="2"/>
-        <v>720</v>
       </c>
       <c r="F8" s="1">
         <v>2</v>
@@ -746,15 +746,15 @@
       </c>
       <c r="C9" s="1">
         <f t="shared" si="1"/>
-        <v>900</v>
+        <v>1125</v>
       </c>
       <c r="D9" s="1">
         <f>C9*1</f>
+        <v>1125</v>
+      </c>
+      <c r="E9" s="1">
+        <f t="shared" si="2"/>
         <v>900</v>
-      </c>
-      <c r="E9" s="1">
-        <f t="shared" si="2"/>
-        <v>720</v>
       </c>
       <c r="F9" s="1">
         <v>2</v>
@@ -775,15 +775,15 @@
       </c>
       <c r="C10" s="1">
         <f t="shared" si="1"/>
-        <v>900</v>
+        <v>1125</v>
       </c>
       <c r="D10" s="1">
         <f>C10*1</f>
+        <v>1125</v>
+      </c>
+      <c r="E10" s="1">
+        <f t="shared" si="2"/>
         <v>900</v>
-      </c>
-      <c r="E10" s="1">
-        <f t="shared" si="2"/>
-        <v>720</v>
       </c>
       <c r="F10" s="1">
         <v>2</v>
@@ -800,19 +800,19 @@
         <v>10</v>
       </c>
       <c r="B11" s="7">
-        <v>585</v>
+        <v>876</v>
       </c>
       <c r="C11" s="1">
         <f t="shared" si="1"/>
-        <v>900</v>
+        <v>1125</v>
       </c>
       <c r="D11" s="1">
         <f>C11</f>
+        <v>1125</v>
+      </c>
+      <c r="E11" s="7">
+        <f t="shared" si="2"/>
         <v>900</v>
-      </c>
-      <c r="E11" s="7">
-        <f t="shared" si="2"/>
-        <v>720</v>
       </c>
       <c r="F11" s="7">
         <v>2</v>
@@ -829,7 +829,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="5">
-        <v>210</v>
+        <v>889</v>
       </c>
       <c r="C12" s="5">
         <f>550*2</f>
@@ -1006,16 +1006,14 @@
         <v>30</v>
       </c>
       <c r="C18" s="1">
-        <f>350*2</f>
-        <v>700</v>
+        <v>1050</v>
       </c>
       <c r="D18" s="5">
-        <f>C18*1</f>
-        <v>700</v>
+        <v>1000</v>
       </c>
       <c r="E18" s="5">
         <f t="shared" si="2"/>
-        <v>560</v>
+        <v>800</v>
       </c>
       <c r="F18" s="5">
         <v>2</v>
@@ -1032,19 +1030,17 @@
         <v>18</v>
       </c>
       <c r="B19" s="1">
-        <v>778</v>
+        <v>116</v>
       </c>
       <c r="C19" s="1">
-        <f t="shared" ref="C19:C26" si="4">350*2</f>
-        <v>700</v>
+        <v>1050</v>
       </c>
       <c r="D19" s="1">
-        <f>C19</f>
-        <v>700</v>
+        <v>1000</v>
       </c>
       <c r="E19" s="1">
         <f t="shared" si="2"/>
-        <v>560</v>
+        <v>800</v>
       </c>
       <c r="F19" s="1">
         <v>2</v>
@@ -1064,16 +1060,14 @@
         <v>614</v>
       </c>
       <c r="C20" s="1">
-        <f t="shared" si="4"/>
-        <v>700</v>
+        <v>1050</v>
       </c>
       <c r="D20" s="1">
-        <f t="shared" ref="D20:D26" si="5">C20</f>
-        <v>700</v>
+        <v>1000</v>
       </c>
       <c r="E20" s="1">
         <f t="shared" si="2"/>
-        <v>560</v>
+        <v>800</v>
       </c>
       <c r="F20" s="1">
         <v>2</v>
@@ -1090,19 +1084,17 @@
         <v>20</v>
       </c>
       <c r="B21" s="1">
-        <v>2180</v>
+        <v>1232</v>
       </c>
       <c r="C21" s="1">
-        <f t="shared" si="4"/>
-        <v>700</v>
+        <v>1050</v>
       </c>
       <c r="D21" s="1">
-        <f t="shared" si="5"/>
-        <v>700</v>
+        <v>1000</v>
       </c>
       <c r="E21" s="1">
         <f t="shared" si="2"/>
-        <v>560</v>
+        <v>800</v>
       </c>
       <c r="F21" s="1">
         <v>2</v>
@@ -1119,19 +1111,17 @@
         <v>21</v>
       </c>
       <c r="B22" s="1">
-        <v>792</v>
+        <v>111</v>
       </c>
       <c r="C22" s="1">
-        <f t="shared" si="4"/>
-        <v>700</v>
+        <v>1050</v>
       </c>
       <c r="D22" s="1">
-        <f t="shared" si="5"/>
-        <v>700</v>
+        <v>1000</v>
       </c>
       <c r="E22" s="1">
         <f t="shared" si="2"/>
-        <v>560</v>
+        <v>800</v>
       </c>
       <c r="F22" s="1">
         <v>2</v>
@@ -1151,16 +1141,14 @@
         <v>274</v>
       </c>
       <c r="C23" s="1">
-        <f t="shared" si="4"/>
         <v>700</v>
       </c>
       <c r="D23" s="1">
-        <f t="shared" si="5"/>
-        <v>700</v>
+        <v>1000</v>
       </c>
       <c r="E23" s="1">
         <f t="shared" si="2"/>
-        <v>560</v>
+        <v>800</v>
       </c>
       <c r="F23" s="1">
         <v>2</v>
@@ -1177,19 +1165,17 @@
         <v>23</v>
       </c>
       <c r="B24" s="1">
-        <v>171</v>
+        <v>685</v>
       </c>
       <c r="C24" s="1">
-        <f t="shared" si="4"/>
         <v>700</v>
       </c>
       <c r="D24" s="1">
-        <f t="shared" si="5"/>
-        <v>700</v>
+        <v>1000</v>
       </c>
       <c r="E24" s="1">
         <f t="shared" si="2"/>
-        <v>560</v>
+        <v>800</v>
       </c>
       <c r="F24" s="1">
         <v>2</v>
@@ -1209,16 +1195,14 @@
         <v>443</v>
       </c>
       <c r="C25" s="1">
-        <f t="shared" si="4"/>
-        <v>700</v>
+        <v>1000</v>
       </c>
       <c r="D25" s="1">
-        <f t="shared" si="5"/>
-        <v>700</v>
+        <v>1000</v>
       </c>
       <c r="E25" s="1">
         <f t="shared" si="2"/>
-        <v>560</v>
+        <v>800</v>
       </c>
       <c r="F25" s="1">
         <v>2</v>
@@ -1231,52 +1215,50 @@
       </c>
     </row>
     <row r="26" spans="1:8" ht="18.75">
-      <c r="A26" s="7">
+      <c r="A26" s="1">
         <v>25</v>
       </c>
       <c r="B26" s="1">
-        <v>1310</v>
+        <v>999</v>
       </c>
       <c r="C26" s="1">
-        <f t="shared" si="4"/>
-        <v>700</v>
-      </c>
-      <c r="D26" s="7">
-        <f t="shared" si="5"/>
-        <v>700</v>
-      </c>
-      <c r="E26" s="7">
-        <f t="shared" si="2"/>
-        <v>560</v>
-      </c>
-      <c r="F26" s="7">
-        <v>2</v>
-      </c>
-      <c r="G26" s="7">
-        <v>3</v>
-      </c>
-      <c r="H26" s="8" t="s">
+        <v>1000</v>
+      </c>
+      <c r="D26" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E26" s="1">
+        <f t="shared" si="2"/>
+        <v>800</v>
+      </c>
+      <c r="F26" s="1">
+        <v>2</v>
+      </c>
+      <c r="G26" s="1">
+        <v>3</v>
+      </c>
+      <c r="H26" s="3" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="18.75">
-      <c r="A27" s="1">
+      <c r="A27" s="5">
         <v>26</v>
       </c>
       <c r="B27" s="5">
         <v>621</v>
       </c>
       <c r="C27" s="5">
-        <f>300*2</f>
-        <v>600</v>
-      </c>
-      <c r="D27" s="1">
+        <f>300*3</f>
+        <v>900</v>
+      </c>
+      <c r="D27" s="5">
         <f>C27*1</f>
-        <v>600</v>
-      </c>
-      <c r="E27" s="1">
-        <f t="shared" si="2"/>
-        <v>480</v>
+        <v>900</v>
+      </c>
+      <c r="E27" s="5">
+        <f t="shared" si="2"/>
+        <v>720</v>
       </c>
       <c r="F27" s="5">
         <v>2</v>
@@ -1296,16 +1278,16 @@
         <v>457</v>
       </c>
       <c r="C28" s="1">
-        <f t="shared" ref="C28:C33" si="6">300*2</f>
-        <v>600</v>
+        <f t="shared" ref="C28:C31" si="4">300*3</f>
+        <v>900</v>
       </c>
       <c r="D28" s="1">
         <f>C28</f>
-        <v>600</v>
+        <v>900</v>
       </c>
       <c r="E28" s="1">
         <f t="shared" si="2"/>
-        <v>480</v>
+        <v>720</v>
       </c>
       <c r="F28" s="1">
         <v>2</v>
@@ -1325,16 +1307,16 @@
         <v>1116</v>
       </c>
       <c r="C29" s="1">
-        <f t="shared" si="6"/>
-        <v>600</v>
+        <f t="shared" si="4"/>
+        <v>900</v>
       </c>
       <c r="D29" s="1">
-        <f t="shared" ref="D29:D33" si="7">C29</f>
-        <v>600</v>
+        <f t="shared" ref="D29:D31" si="5">C29</f>
+        <v>900</v>
       </c>
       <c r="E29" s="1">
         <f t="shared" si="2"/>
-        <v>480</v>
+        <v>720</v>
       </c>
       <c r="F29" s="1">
         <v>2</v>
@@ -1351,19 +1333,19 @@
         <v>29</v>
       </c>
       <c r="B30" s="1">
-        <v>1306</v>
+        <v>152</v>
       </c>
       <c r="C30" s="1">
-        <f t="shared" si="6"/>
-        <v>600</v>
+        <f t="shared" si="4"/>
+        <v>900</v>
       </c>
       <c r="D30" s="1">
-        <f t="shared" si="7"/>
-        <v>600</v>
+        <f t="shared" si="5"/>
+        <v>900</v>
       </c>
       <c r="E30" s="1">
         <f t="shared" si="2"/>
-        <v>480</v>
+        <v>720</v>
       </c>
       <c r="F30" s="1">
         <v>2</v>
@@ -1380,19 +1362,19 @@
         <v>30</v>
       </c>
       <c r="B31" s="1">
-        <v>1062</v>
+        <v>650</v>
       </c>
       <c r="C31" s="1">
-        <f t="shared" si="6"/>
-        <v>600</v>
+        <f t="shared" si="4"/>
+        <v>900</v>
       </c>
       <c r="D31" s="1">
-        <f t="shared" si="7"/>
-        <v>600</v>
+        <f t="shared" si="5"/>
+        <v>900</v>
       </c>
       <c r="E31" s="1">
         <f t="shared" si="2"/>
-        <v>480</v>
+        <v>720</v>
       </c>
       <c r="F31" s="1">
         <v>2</v>
@@ -1409,19 +1391,17 @@
         <v>31</v>
       </c>
       <c r="B32" s="1">
-        <v>1089</v>
+        <v>58</v>
       </c>
       <c r="C32" s="1">
-        <f t="shared" si="6"/>
         <v>600</v>
       </c>
       <c r="D32" s="1">
-        <f t="shared" si="7"/>
-        <v>600</v>
+        <v>900</v>
       </c>
       <c r="E32" s="1">
         <f t="shared" si="2"/>
-        <v>480</v>
+        <v>720</v>
       </c>
       <c r="F32" s="1">
         <v>2</v>
@@ -1441,16 +1421,14 @@
         <v>383</v>
       </c>
       <c r="C33" s="7">
-        <f t="shared" si="6"/>
         <v>600</v>
       </c>
       <c r="D33" s="7">
-        <f t="shared" si="7"/>
-        <v>600</v>
+        <v>900</v>
       </c>
       <c r="E33" s="7">
         <f t="shared" si="2"/>
-        <v>480</v>
+        <v>720</v>
       </c>
       <c r="F33" s="7">
         <v>2</v>
@@ -1473,8 +1451,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC549F17-0A38-47FF-88AF-64A96651F191}">
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1526,7 +1504,7 @@
         <v>675</v>
       </c>
       <c r="D2" s="1">
-        <f t="shared" ref="D2:D14" si="0">C2*0.8</f>
+        <f t="shared" ref="D2:D10" si="0">C2*0.8</f>
         <v>540</v>
       </c>
       <c r="E2" s="1">
@@ -1557,7 +1535,7 @@
         <v>283</v>
       </c>
       <c r="C3" s="1">
-        <f t="shared" ref="C3:C8" si="1">300*1.5*1.5</f>
+        <f t="shared" ref="C3:C7" si="1">300*1.5*1.5</f>
         <v>675</v>
       </c>
       <c r="D3" s="1">
@@ -1732,28 +1710,27 @@
         <v>652</v>
       </c>
       <c r="C8" s="1">
-        <f t="shared" si="1"/>
-        <v>675</v>
+        <v>450</v>
       </c>
       <c r="D8" s="1">
         <f t="shared" si="0"/>
-        <v>540</v>
+        <v>360</v>
       </c>
       <c r="E8" s="1">
         <f t="shared" si="2"/>
-        <v>472.49999999999994</v>
+        <v>315</v>
       </c>
       <c r="F8" s="1">
         <f t="shared" si="3"/>
-        <v>1350</v>
+        <v>900</v>
       </c>
       <c r="G8" s="1">
         <f t="shared" si="4"/>
-        <v>135</v>
+        <v>90</v>
       </c>
       <c r="H8" s="1">
         <f t="shared" si="5"/>
-        <v>675</v>
+        <v>450</v>
       </c>
       <c r="I8" s="1">
         <v>3</v>
@@ -1764,7 +1741,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="1">
-        <v>1103</v>
+        <v>426</v>
       </c>
       <c r="C9" s="1">
         <f>450</f>
@@ -1799,31 +1776,30 @@
         <v>9</v>
       </c>
       <c r="B10" s="1">
-        <v>1462</v>
+        <v>820</v>
       </c>
       <c r="C10" s="1">
-        <f>450</f>
-        <v>450</v>
+        <v>675</v>
       </c>
       <c r="D10" s="1">
         <f t="shared" si="0"/>
-        <v>360</v>
+        <v>540</v>
       </c>
       <c r="E10" s="1">
         <f t="shared" si="2"/>
-        <v>315</v>
+        <v>472.49999999999994</v>
       </c>
       <c r="F10" s="1">
         <f t="shared" si="3"/>
-        <v>900</v>
+        <v>1350</v>
       </c>
       <c r="G10" s="1">
         <f t="shared" si="4"/>
-        <v>90</v>
+        <v>135</v>
       </c>
       <c r="H10" s="1">
         <f t="shared" si="5"/>
-        <v>450</v>
+        <v>675</v>
       </c>
       <c r="I10" s="1">
         <v>3</v>
@@ -1834,31 +1810,30 @@
         <v>10</v>
       </c>
       <c r="B11" s="1">
-        <v>745</v>
+        <v>443</v>
       </c>
       <c r="C11" s="1">
-        <f>450</f>
-        <v>450</v>
+        <v>675</v>
       </c>
       <c r="D11" s="1">
-        <f t="shared" si="0"/>
-        <v>360</v>
+        <f>C11*0.8</f>
+        <v>540</v>
       </c>
       <c r="E11" s="1">
         <f t="shared" si="2"/>
-        <v>315</v>
+        <v>472.49999999999994</v>
       </c>
       <c r="F11" s="1">
         <f t="shared" si="3"/>
-        <v>900</v>
+        <v>1350</v>
       </c>
       <c r="G11" s="1">
         <f t="shared" si="4"/>
-        <v>90</v>
+        <v>135</v>
       </c>
       <c r="H11" s="1">
         <f t="shared" si="5"/>
-        <v>450</v>
+        <v>675</v>
       </c>
       <c r="I11" s="1">
         <v>3</v>
@@ -1869,31 +1844,30 @@
         <v>11</v>
       </c>
       <c r="B12" s="1">
-        <v>1487</v>
+        <v>1161</v>
       </c>
       <c r="C12" s="1">
-        <f>450</f>
-        <v>450</v>
+        <v>675</v>
       </c>
       <c r="D12" s="1">
-        <f t="shared" si="0"/>
-        <v>360</v>
+        <f t="shared" ref="D12:D14" si="6">C12*0.8</f>
+        <v>540</v>
       </c>
       <c r="E12" s="1">
         <f t="shared" si="2"/>
-        <v>315</v>
+        <v>472.49999999999994</v>
       </c>
       <c r="F12" s="1">
         <f t="shared" si="3"/>
-        <v>900</v>
+        <v>1350</v>
       </c>
       <c r="G12" s="1">
         <f t="shared" si="4"/>
-        <v>90</v>
+        <v>135</v>
       </c>
       <c r="H12" s="1">
         <f t="shared" si="5"/>
-        <v>450</v>
+        <v>675</v>
       </c>
       <c r="I12" s="1">
         <v>3</v>
@@ -1907,28 +1881,27 @@
         <v>1484</v>
       </c>
       <c r="C13" s="1">
-        <f>450</f>
-        <v>450</v>
+        <v>675</v>
       </c>
       <c r="D13" s="1">
-        <f t="shared" si="0"/>
-        <v>360</v>
+        <f t="shared" si="6"/>
+        <v>540</v>
       </c>
       <c r="E13" s="1">
         <f t="shared" si="2"/>
-        <v>315</v>
+        <v>472.49999999999994</v>
       </c>
       <c r="F13" s="1">
         <f t="shared" si="3"/>
-        <v>900</v>
+        <v>1350</v>
       </c>
       <c r="G13" s="1">
         <f t="shared" si="4"/>
-        <v>90</v>
+        <v>135</v>
       </c>
       <c r="H13" s="1">
         <f t="shared" si="5"/>
-        <v>450</v>
+        <v>675</v>
       </c>
       <c r="I13" s="1">
         <v>4</v>
@@ -1939,31 +1912,30 @@
         <v>13</v>
       </c>
       <c r="B14" s="1">
-        <v>1062</v>
+        <v>353</v>
       </c>
       <c r="C14" s="1">
-        <f>450</f>
-        <v>450</v>
+        <v>675</v>
       </c>
       <c r="D14" s="1">
-        <f t="shared" si="0"/>
-        <v>360</v>
+        <f t="shared" si="6"/>
+        <v>540</v>
       </c>
       <c r="E14" s="1">
         <f>C14*0.7</f>
-        <v>315</v>
+        <v>472.49999999999994</v>
       </c>
       <c r="F14" s="1">
         <f t="shared" si="3"/>
-        <v>900</v>
+        <v>1350</v>
       </c>
       <c r="G14" s="1">
         <f t="shared" si="4"/>
-        <v>90</v>
+        <v>135</v>
       </c>
       <c r="H14" s="1">
         <f t="shared" si="5"/>
-        <v>450</v>
+        <v>675</v>
       </c>
       <c r="I14" s="1">
         <v>4</v>
@@ -1981,7 +1953,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -2035,7 +2007,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>733</v>
+        <v>232</v>
       </c>
       <c r="C3" s="2">
         <f>3000</f>
@@ -2111,7 +2083,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1">
-        <v>244</v>
+        <v>279</v>
       </c>
       <c r="C7" s="1">
         <f>1000</f>
@@ -2130,7 +2102,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="1">
-        <v>49</v>
+        <v>653</v>
       </c>
       <c r="C8" s="1">
         <f>500</f>
@@ -2149,7 +2121,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="1">
-        <v>92</v>
+        <v>110</v>
       </c>
       <c r="C9" s="1">
         <f>500</f>
@@ -2168,7 +2140,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="1">
-        <v>1153</v>
+        <v>820</v>
       </c>
       <c r="C10" s="1">
         <f>500</f>
@@ -2187,7 +2159,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="1">
-        <v>578</v>
+        <v>1396</v>
       </c>
       <c r="C11" s="1">
         <f>500</f>
@@ -2206,7 +2178,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="1">
-        <v>863</v>
+        <v>94</v>
       </c>
       <c r="C12" s="1">
         <f>1000</f>
@@ -2244,7 +2216,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="1">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="C14" s="1">
         <v>1000</v>
@@ -2262,7 +2234,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="1">
-        <v>58</v>
+        <v>488</v>
       </c>
       <c r="C15" s="1">
         <f>500</f>
@@ -2281,7 +2253,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="1">
-        <v>601</v>
+        <v>354</v>
       </c>
       <c r="C16" s="1">
         <f>500</f>

</xml_diff>